<commit_message>
Added IP address for Radius server
</commit_message>
<xml_diff>
--- a/IPAddressScheme.xlsx
+++ b/IPAddressScheme.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="85">
   <si>
     <t>VLAN</t>
   </si>
@@ -258,6 +258,27 @@
   </si>
   <si>
     <t>97.168.90.103</t>
+  </si>
+  <si>
+    <t>Radius Server</t>
+  </si>
+  <si>
+    <t>172.16.8.224</t>
+  </si>
+  <si>
+    <t>172.16.8.225</t>
+  </si>
+  <si>
+    <t>/30</t>
+  </si>
+  <si>
+    <t>255.255.255.252</t>
+  </si>
+  <si>
+    <t>172.16.8.226</t>
+  </si>
+  <si>
+    <t>172.16.8.227</t>
   </si>
 </sst>
 </file>
@@ -575,10 +596,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J13"/>
+  <dimension ref="A1:J14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -948,40 +969,43 @@
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A12">
+        <v>1</v>
+      </c>
       <c r="B12" t="s">
-        <v>68</v>
+        <v>78</v>
       </c>
       <c r="C12" t="s">
-        <v>70</v>
+        <v>79</v>
       </c>
       <c r="D12" t="s">
-        <v>47</v>
+        <v>81</v>
       </c>
       <c r="E12" t="s">
-        <v>48</v>
+        <v>82</v>
       </c>
       <c r="F12" t="s">
-        <v>71</v>
+        <v>80</v>
       </c>
       <c r="G12" t="s">
-        <v>72</v>
+        <v>83</v>
       </c>
       <c r="H12" t="s">
-        <v>73</v>
+        <v>84</v>
       </c>
       <c r="I12">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="J12">
-        <v>6</v>
+        <v>2</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.35">
       <c r="B13" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C13" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="D13" t="s">
         <v>47</v>
@@ -990,18 +1014,47 @@
         <v>48</v>
       </c>
       <c r="F13" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="G13" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="H13" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="I13">
         <v>3</v>
       </c>
       <c r="J13">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="B14" t="s">
+        <v>69</v>
+      </c>
+      <c r="C14" t="s">
+        <v>74</v>
+      </c>
+      <c r="D14" t="s">
+        <v>47</v>
+      </c>
+      <c r="E14" t="s">
+        <v>48</v>
+      </c>
+      <c r="F14" t="s">
+        <v>75</v>
+      </c>
+      <c r="G14" t="s">
+        <v>76</v>
+      </c>
+      <c r="H14" t="s">
+        <v>77</v>
+      </c>
+      <c r="I14">
+        <v>3</v>
+      </c>
+      <c r="J14">
         <v>6</v>
       </c>
     </row>

</xml_diff>